<commit_message>
Bugfix: Credible intervals illustrative examples
Mistakenly used confidence intervals instead of credible intervals for illustrative examples (both statistics).
</commit_message>
<xml_diff>
--- a/ldm_t/applied_examples.xlsx
+++ b/ldm_t/applied_examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\GitHub\ACE\ldm_t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33AB9A1-970C-47F1-A5E7-5C9FE8A44DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5487DF15-1A91-4DFF-B813-B2429EF11F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="2160" windowWidth="20970" windowHeight="12150" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
+    <workbookView xWindow="3795" yWindow="3585" windowWidth="20970" windowHeight="12150" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chol Crit" sheetId="6" r:id="rId1"/>
@@ -1785,7 +1785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2043,12 +2043,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="286">
+  <dxfs count="287">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4361,1455 +4371,1504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72E46EB-EFC0-49AE-9709-D9D6BDFCCEF6}">
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="4.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="4.140625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="5.7109375" style="5" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" style="5" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="1" customWidth="1"/>
-    <col min="21" max="22" width="4.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="5.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="4.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="4.28515625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="6.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="3.85546875" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="4.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" style="5" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="5" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" style="5" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="4.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="4.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.5703125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:24" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="93"/>
+      <c r="B2" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="C2" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="D2" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="E2" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="F2" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="G2" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="H2" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="I2" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="K2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="L2" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="M2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="N2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="O2" s="33"/>
       <c r="P2" s="33"/>
       <c r="Q2" s="33"/>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
-    </row>
-    <row r="3" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="T2" s="33"/>
+    </row>
+    <row r="3" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
         <v>-0.30037453183520602</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>1335</v>
       </c>
-      <c r="D3" s="12">
-        <f>(1430-C3)*SQRT(E3)</f>
+      <c r="E3" s="12">
+        <f>(1430-D3)*SQRT(F3)</f>
         <v>268.70057685088807</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>934</v>
       </c>
-      <c r="H3" s="2">
-        <f>(G3-852)*SQRT(I3)</f>
+      <c r="I3" s="2">
+        <f>(H3-852)*SQRT(J3)</f>
         <v>231.93102422918761</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>8</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="K3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>-2.4844186767257598E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:24" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
         <v>-0.33069306930693099</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>202</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <f>12.59</f>
         <v>12.59</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>135.19999999999999</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <f>28.72</f>
         <v>28.72</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>5</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>-6.6189329278212194E-2</v>
       </c>
-      <c r="O4" s="38"/>
       <c r="P4" s="38"/>
       <c r="Q4" s="38"/>
       <c r="R4" s="38"/>
       <c r="S4" s="38"/>
-    </row>
-    <row r="5" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="T4" s="38"/>
+    </row>
+    <row r="5" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="29">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>-0.20735117858569699</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>2503</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>266</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>1984</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>252</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>13</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>0.05</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>-0.134886230157099</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:24" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
         <v>-0.45140388768898498</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>463</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>103</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>254</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>108</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>10</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N6" s="23">
+      <c r="O6" s="23">
         <v>-0.13934928786244699</v>
       </c>
-      <c r="O6" s="38"/>
       <c r="P6" s="38"/>
       <c r="Q6" s="38"/>
       <c r="R6" s="38"/>
       <c r="S6" s="38"/>
-    </row>
-    <row r="7" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="T6" s="38"/>
+    </row>
+    <row r="7" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26">
         <v>-0.28749401054144702</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="C7" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="43">
+      <c r="D7" s="43">
         <v>2087</v>
       </c>
-      <c r="D7" s="44">
+      <c r="E7" s="44">
         <v>530.59871843041617</v>
       </c>
-      <c r="E7" s="28">
+      <c r="F7" s="28">
         <v>15</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="G7" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="43">
+      <c r="H7" s="43">
         <v>1487</v>
       </c>
-      <c r="H7" s="28">
+      <c r="I7" s="28">
         <v>364</v>
       </c>
-      <c r="I7" s="28">
+      <c r="J7" s="28">
         <v>16</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="K7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="28">
+      <c r="L7" s="28">
         <v>0.05</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="M7" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="M7" s="45" t="s">
+      <c r="N7" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="29">
+      <c r="O7" s="29">
         <v>-0.16428051608425101</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
+    <row r="8" spans="1:24" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26">
         <v>-0.35714285714285698</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="C8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="28">
         <v>238</v>
       </c>
-      <c r="D8" s="28">
-        <f>(245-C8)*SQRT(E8)</f>
+      <c r="E8" s="28">
+        <f>(245-D8)*SQRT(F8)</f>
         <v>15.652475842498529</v>
       </c>
-      <c r="E8" s="28">
+      <c r="F8" s="28">
         <v>5</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="G8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="28">
+      <c r="H8" s="28">
         <v>153</v>
       </c>
-      <c r="H8" s="39">
-        <f>(163-G8)*SQRT(I8)</f>
+      <c r="I8" s="39">
+        <f>(163-H8)*SQRT(J8)</f>
         <v>22.360679774997898</v>
       </c>
-      <c r="I8" s="28">
+      <c r="J8" s="28">
         <v>5</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="K8" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="L8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="M8" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="N8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="29">
+      <c r="O8" s="29">
         <v>-0.17134575423015799</v>
       </c>
-      <c r="O8" s="38"/>
       <c r="P8" s="38"/>
       <c r="Q8" s="38"/>
       <c r="R8" s="38"/>
       <c r="S8" s="38"/>
-    </row>
-    <row r="9" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
+      <c r="T8" s="38"/>
+    </row>
+    <row r="9" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>7</v>
+      </c>
+      <c r="B9" s="26">
         <v>-0.30962343096234302</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="C9" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="28">
         <v>4.78</v>
       </c>
-      <c r="D9" s="28">
-        <f>(5.05-4.78)*SQRT(E9)</f>
+      <c r="E9" s="28">
+        <f>(5.05-4.78)*SQRT(F9)</f>
         <v>1.2074767078498845</v>
       </c>
-      <c r="E9" s="28">
+      <c r="F9" s="28">
         <v>20</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="G9" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="28">
+      <c r="H9" s="28">
         <v>3.3</v>
       </c>
-      <c r="H9" s="41">
-        <f>(3.45-G9)*SQRT(I9)</f>
+      <c r="I9" s="41">
+        <f>(3.45-H9)*SQRT(J9)</f>
         <v>0.67082039324993858</v>
       </c>
-      <c r="I9" s="28">
+      <c r="J9" s="28">
         <v>20</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="K9" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="L9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="M9" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="M9" s="29" t="s">
+      <c r="N9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="29">
+      <c r="O9" s="29">
         <v>-0.17471020283654001</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="10" spans="1:24" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
         <v>-0.30962343096234302</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>4.78</v>
       </c>
-      <c r="D10" s="2">
-        <f>(5.05-4.78)*SQRT(E10)</f>
+      <c r="E10" s="2">
+        <f>(5.05-4.78)*SQRT(F10)</f>
         <v>1.2074767078498845</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>20</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>3.3</v>
       </c>
-      <c r="H10" s="2">
-        <f>(3.45-G10)*SQRT(I10)</f>
+      <c r="I10" s="2">
+        <f>(3.45-H10)*SQRT(J10)</f>
         <v>0.67082039324993858</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>20</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="K10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>-0.17477379644529401</v>
       </c>
-      <c r="O10" s="38"/>
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
       <c r="R10" s="38"/>
       <c r="S10" s="38"/>
-    </row>
-    <row r="11" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="T10" s="38"/>
+    </row>
+    <row r="11" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
         <v>-0.45140388768898498</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>463</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>103</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>12</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>254</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>108</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>10</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>0.05</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>-0.295786280202745</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <f>(G12-C12)/C12</f>
+    <row r="12" spans="1:24" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <f>(H12-D12)/D12</f>
         <v>-0.51619644723093006</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>95.7</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>9.4</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>46.3</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>1.9</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>4</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>0.05</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>-0.44201349509253401</v>
       </c>
-      <c r="O12" s="37"/>
       <c r="P12" s="37"/>
       <c r="Q12" s="37"/>
       <c r="R12" s="37"/>
       <c r="S12" s="37"/>
-    </row>
-    <row r="13" spans="1:23" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="T12" s="37"/>
+    </row>
+    <row r="13" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
         <v>-0.57999999999999996</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>300</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>97</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>13</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>126</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>41</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>14</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>0.05</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>-0.46949572295293701</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="26">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
+        <v>12</v>
+      </c>
+      <c r="B14" s="26">
         <v>-0.55919003115264798</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="C14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="28">
+      <c r="D14" s="28">
         <v>642</v>
       </c>
-      <c r="D14" s="28">
+      <c r="E14" s="28">
         <v>63</v>
       </c>
-      <c r="E14" s="28">
+      <c r="F14" s="28">
         <v>9</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="G14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="28">
+      <c r="H14" s="28">
         <v>283</v>
       </c>
-      <c r="H14" s="28">
+      <c r="I14" s="28">
         <v>69</v>
       </c>
-      <c r="I14" s="28">
+      <c r="J14" s="28">
         <v>10</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="K14" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="28">
+      <c r="L14" s="28">
         <v>0.05</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="M14" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="M14" s="27" t="s">
+      <c r="N14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="29">
+      <c r="O14" s="29">
         <v>-0.48827479402393598</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <f>(G15-C15)/C15</f>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <f>(H15-D15)/D15</f>
         <v>-0.69333979352241815</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="12">
+      <c r="D15" s="12">
         <v>268.31</v>
       </c>
-      <c r="D15" s="14">
+      <c r="E15" s="14">
         <v>53.83</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>6</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G15" s="14">
+      <c r="H15" s="14">
         <v>82.28</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>30.7</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>10</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>-0.537663083644214</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <f>(G16-C16)/C16</f>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <f>(H16-D16)/D16</f>
         <v>-0.81742738589211617</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>241</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10</v>
       </c>
       <c r="E16" s="2">
         <v>10</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>44</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>15</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>5</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>-0.70784557884844101</v>
       </c>
-      <c r="W16" s="5"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="W17" s="5"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="J19" s="13"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="J20" s="13"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-      <c r="D22" s="12"/>
-      <c r="F22" s="1"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="15"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="X16" s="5"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="X17" s="5"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="K19" s="13"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="K20" s="13"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="5"/>
+      <c r="E22" s="12"/>
+      <c r="G22" s="1"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:24" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B34" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="G34" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="J34" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="K34" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="L34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="M34" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="M34" s="9" t="s">
+      <c r="N34" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <f t="shared" ref="A35:A42" si="0">(G35-C35)/C35</f>
+    <row r="35" spans="2:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="3">
+        <f t="shared" ref="B35:B42" si="0">(H35-D35)/D35</f>
         <v>-0.28749401054144708</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="11">
+      <c r="D35" s="11">
         <v>2087</v>
       </c>
-      <c r="D35" s="12">
+      <c r="E35" s="12">
         <v>530.59871843041617</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>15</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="G35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="11">
+      <c r="H35" s="11">
         <v>1487</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>364</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>16</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K35" s="2">
+      <c r="L35" s="2">
         <v>0.05</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="M35" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="N35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3">
         <f t="shared" si="0"/>
         <v>0.40384615384615385</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="2">
+      <c r="D36" s="2">
         <v>104</v>
       </c>
-      <c r="D36" s="2">
+      <c r="E36" s="2">
         <v>16</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>8</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="G36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="2">
+      <c r="H36" s="2">
         <v>146</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>34</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>9</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K36" s="2">
+      <c r="L36" s="2">
         <v>0.05</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="N36" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="37" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="3">
         <f t="shared" si="0"/>
         <v>0.35576923076923078</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="2">
+      <c r="D37" s="2">
         <v>104</v>
       </c>
-      <c r="D37" s="2">
+      <c r="E37" s="2">
         <v>16</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="2">
         <v>8</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G37" s="2">
+      <c r="H37" s="2">
         <v>141</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>34</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>8</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K37" s="2">
+      <c r="L37" s="2">
         <v>0.05</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="M37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="N37" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+    <row r="38" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3">
         <f t="shared" si="0"/>
         <v>-0.20735117858569715</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="2">
+      <c r="D38" s="2">
         <v>2503</v>
       </c>
-      <c r="D38" s="2">
+      <c r="E38" s="2">
         <v>266</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="2">
         <v>11</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G38" s="2">
+      <c r="H38" s="2">
         <v>1984</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>252</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>13</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
         <v>0.05</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M38" s="4" t="s">
+      <c r="N38" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    <row r="39" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="3">
         <f t="shared" si="0"/>
         <v>-0.55919003115264798</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="2">
+      <c r="D39" s="2">
         <v>642</v>
       </c>
-      <c r="D39" s="2">
+      <c r="E39" s="2">
         <v>63</v>
       </c>
-      <c r="E39" s="2">
+      <c r="F39" s="2">
         <v>9</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>283</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>69</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>10</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K39" s="2">
+      <c r="L39" s="2">
         <v>0.05</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="N39" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="40" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3">
         <f t="shared" si="0"/>
         <v>-0.57999999999999996</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="2">
+      <c r="D40" s="2">
         <v>300</v>
       </c>
-      <c r="D40" s="2">
+      <c r="E40" s="2">
         <v>97</v>
       </c>
-      <c r="E40" s="2">
+      <c r="F40" s="2">
         <v>13</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="G40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="2">
+      <c r="H40" s="2">
         <v>126</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>41</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>14</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="2">
+      <c r="L40" s="2">
         <v>0.05</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="N40" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="41" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3">
         <f t="shared" si="0"/>
         <v>-0.45140388768898487</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="2">
+      <c r="D41" s="2">
         <v>463</v>
       </c>
-      <c r="D41" s="2">
+      <c r="E41" s="2">
         <v>103</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="2">
         <v>12</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="2">
+      <c r="H41" s="2">
         <v>254</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>108</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>10</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="L41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="M41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+    <row r="42" spans="2:20" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="3">
         <f t="shared" si="0"/>
         <v>0.30452674897119331</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="2">
+      <c r="D42" s="2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="D42" s="2">
+      <c r="E42" s="2">
         <v>0.7103520254071215</v>
       </c>
-      <c r="E42" s="2">
+      <c r="F42" s="2">
         <v>6</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H42" s="2">
         <v>3.17</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>0.51961524227066314</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>12</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="K42" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K42" s="2">
+      <c r="L42" s="2">
         <v>0.05</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="M42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <f>(G43-C43)/C43</f>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B43" s="3">
+        <f>(H43-D43)/D43</f>
         <v>-0.35714285714285715</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="2">
+      <c r="D43" s="2">
         <v>238</v>
       </c>
-      <c r="D43" s="2">
-        <f>(245-C43)*SQRT(E43)</f>
+      <c r="E43" s="2">
+        <f>(245-D43)*SQRT(F43)</f>
         <v>15.652475842498529</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="2">
         <v>5</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="2">
+      <c r="H43" s="2">
         <v>153</v>
       </c>
-      <c r="H43" s="2">
-        <f>(163-G43)*SQRT(I43)</f>
+      <c r="I43" s="2">
+        <f>(163-H43)*SQRT(J43)</f>
         <v>22.360679774997898</v>
       </c>
-      <c r="I43" s="2">
+      <c r="J43" s="2">
         <v>5</v>
       </c>
-      <c r="J43" s="13" t="s">
+      <c r="K43" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <f>(G44-C44)/C44</f>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B44" s="3">
+        <f>(H44-D44)/D44</f>
         <v>-0.30962343096234318</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="2">
+      <c r="D44" s="2">
         <v>4.78</v>
       </c>
-      <c r="D44" s="2">
-        <f>(5.05-4.78)*SQRT(E44)</f>
+      <c r="E44" s="2">
+        <f>(5.05-4.78)*SQRT(F44)</f>
         <v>1.2074767078498845</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="2">
         <v>20</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G44" s="2">
+      <c r="H44" s="2">
         <v>3.3</v>
       </c>
-      <c r="H44" s="2">
-        <f>(3.45-G44)*SQRT(I44)</f>
+      <c r="I44" s="2">
+        <f>(3.45-H44)*SQRT(J44)</f>
         <v>0.67082039324993858</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>20</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="K44" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="M44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <f>(G45-C45)/C45</f>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B45" s="3">
+        <f>(H45-D45)/D45</f>
         <v>-0.30037453183520602</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="2">
+      <c r="D45" s="2">
         <v>1335</v>
       </c>
-      <c r="D45" s="12">
-        <f>(1430-C45)*SQRT(E45)</f>
+      <c r="E45" s="12">
+        <f>(1430-D45)*SQRT(F45)</f>
         <v>268.70057685088807</v>
       </c>
-      <c r="E45" s="2">
+      <c r="F45" s="2">
         <v>8</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G45" s="2">
+      <c r="H45" s="2">
         <v>934</v>
       </c>
-      <c r="H45" s="2">
-        <f>(G45-852)*SQRT(I45)</f>
+      <c r="I45" s="2">
+        <f>(H45-852)*SQRT(J45)</f>
         <v>231.93102422918761</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>8</v>
       </c>
-      <c r="J45" s="13" t="s">
+      <c r="K45" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="M45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="N45" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <f>(G46-C46)/C46</f>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B46" s="3">
+        <f>(H46-D46)/D46</f>
         <v>-0.33069306930693076</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="2">
+      <c r="D46" s="2">
         <v>202</v>
       </c>
-      <c r="D46" s="2">
-        <f>12.59*SQRT(E46)</f>
+      <c r="E46" s="2">
+        <f>12.59*SQRT(F46)</f>
         <v>28.152095836722353</v>
       </c>
-      <c r="E46" s="2">
+      <c r="F46" s="2">
         <v>5</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G46" s="2">
+      <c r="H46" s="2">
         <v>135.19999999999999</v>
       </c>
-      <c r="H46" s="2">
-        <f>28.72*SQRT(I46)</f>
+      <c r="I46" s="2">
+        <f>28.72*SQRT(J46)</f>
         <v>64.219872313793957</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>5</v>
       </c>
-      <c r="J46" s="13" t="s">
+      <c r="K46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="M46" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="N46" s="4" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N16">
-    <sortCondition descending="1" ref="N3:N16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O16">
+    <sortCondition descending="1" ref="O3:O16"/>
   </sortState>
-  <conditionalFormatting sqref="Q7:XFD7 N7:O7 Q13:XFD13 N2:XFD6 AB35:XFD35 N13:O13 A31:I31 K31:M31 A34:M44 B1:XFD1 N8:XFD12 A35:O35 A3:M9 A2 J2:M2 A22:M23 A32:XFD34 A36:XFD1048576 N18:XFD31 N17:R17 T17:V17 N14:XFD16 X17:XFD17 A12:M20">
-    <cfRule type="expression" dxfId="285" priority="45">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="284" priority="46">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45:D45">
-    <cfRule type="expression" dxfId="283" priority="21">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="282" priority="22">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M45">
-    <cfRule type="expression" dxfId="281" priority="19">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="280" priority="20">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="expression" dxfId="279" priority="17">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="278" priority="18">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A10 E10:L10 A11:M11">
-    <cfRule type="expression" dxfId="277" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="276" priority="14">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:D10">
-    <cfRule type="expression" dxfId="275" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="274" priority="12">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="expression" dxfId="273" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="272" priority="10">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I2">
-    <cfRule type="expression" dxfId="271" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="270" priority="8">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:D22">
-    <cfRule type="expression" dxfId="269" priority="3">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="268" priority="4">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M22">
-    <cfRule type="expression" dxfId="267" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="266" priority="2">
-      <formula>"MOD(ROW(),2)=0"</formula>
+  <conditionalFormatting sqref="R7:XFD7 O7:P7 R13:XFD13 O2:XFD6 AC35:XFD35 O13:P13 B31:J31 L31:N31 B34:N44 C1:XFD1 O8:XFD12 B35:P35 B3:N9 B2 K2:N2 B22:N23 A32:XFD34 A36:XFD1048576 O18:XFD31 O17:S17 U17:W17 O14:XFD16 Y17:XFD17 B12:N20">
+    <cfRule type="expression" dxfId="286" priority="46">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="285" priority="47">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:E45">
+    <cfRule type="expression" dxfId="284" priority="22">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="283" priority="23">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N45">
+    <cfRule type="expression" dxfId="282" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="281" priority="21">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="expression" dxfId="280" priority="18">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="279" priority="19">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10 F10:M10 B11:N11">
+    <cfRule type="expression" dxfId="278" priority="14">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="277" priority="15">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="expression" dxfId="276" priority="12">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="275" priority="13">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10">
+    <cfRule type="expression" dxfId="274" priority="10">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="273" priority="11">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:J2">
+    <cfRule type="expression" dxfId="272" priority="8">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="271" priority="9">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:E22">
+    <cfRule type="expression" dxfId="270" priority="4">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="269" priority="5">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N22">
+    <cfRule type="expression" dxfId="268" priority="2">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="267" priority="3">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6355,13 +6414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5AD335-144A-41B4-9F3B-21F68DE79361}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N16"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="2" customWidth="1"/>
@@ -6399,7 +6458,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="47" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="93"/>
       <c r="B2" s="36" t="s">
         <v>113</v>
       </c>
@@ -6492,7 +6551,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29">
+      <c r="A4" s="23">
         <v>2</v>
       </c>
       <c r="B4" s="25">
@@ -6590,7 +6649,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+      <c r="A6" s="23">
         <v>4</v>
       </c>
       <c r="B6" s="3">
@@ -6691,7 +6750,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="A8" s="23">
         <v>6</v>
       </c>
       <c r="B8" s="25">
@@ -6790,7 +6849,7 @@
       <c r="P9" s="29"/>
     </row>
     <row r="10" spans="1:16" s="50" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
+      <c r="A10" s="23">
         <v>8</v>
       </c>
       <c r="B10" s="3">
@@ -6886,7 +6945,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
+      <c r="A12" s="23">
         <v>10</v>
       </c>
       <c r="B12" s="25">
@@ -6984,7 +7043,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="29">
+      <c r="A14" s="23">
         <v>12</v>
       </c>
       <c r="B14" s="3">
@@ -7080,7 +7139,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="29">
+      <c r="A16" s="23">
         <v>14</v>
       </c>
       <c r="B16" s="3">
@@ -8119,1070 +8178,1070 @@
     <sortCondition descending="1" ref="O3:O16"/>
   </sortState>
   <conditionalFormatting sqref="Q9:XFD9 Q15:XFD15 AB31:XFD31 B2 O29:XFD30 O31 K2:N2 O32:XFD33 B19:N20 A1:XFD1 A34:XFD1048576 O2:XFD3 B9:N16 B28:O28 P4:XFD8 P10:XFD14 O17:XFD27 P16:XFD16 O4:O16">
-    <cfRule type="expression" dxfId="265" priority="359">
+    <cfRule type="expression" dxfId="266" priority="359">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1 B20 B13 B3 B27">
-    <cfRule type="expression" dxfId="264" priority="349">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="263" priority="350">
+    <cfRule type="expression" dxfId="265" priority="349">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="264" priority="350">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37 E37:L37 N37">
-    <cfRule type="expression" dxfId="262" priority="347">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="261" priority="348">
+    <cfRule type="expression" dxfId="263" priority="347">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="262" priority="348">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38">
-    <cfRule type="expression" dxfId="260" priority="345">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="259" priority="346">
+    <cfRule type="expression" dxfId="261" priority="345">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="260" priority="346">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39">
-    <cfRule type="expression" dxfId="258" priority="343">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="257" priority="344">
+    <cfRule type="expression" dxfId="259" priority="343">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="258" priority="344">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40">
-    <cfRule type="expression" dxfId="256" priority="341">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="255" priority="342">
+    <cfRule type="expression" dxfId="257" priority="341">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="256" priority="342">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42">
-    <cfRule type="expression" dxfId="254" priority="337">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="253" priority="338">
+    <cfRule type="expression" dxfId="255" priority="337">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="254" priority="338">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43">
-    <cfRule type="expression" dxfId="252" priority="335">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="251" priority="336">
+    <cfRule type="expression" dxfId="253" priority="335">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="252" priority="336">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="expression" dxfId="250" priority="323">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="249" priority="324">
+    <cfRule type="expression" dxfId="251" priority="323">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="250" priority="324">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="248" priority="331">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="247" priority="332">
+    <cfRule type="expression" dxfId="249" priority="331">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="248" priority="332">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="expression" dxfId="246" priority="329">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="245" priority="330">
+    <cfRule type="expression" dxfId="247" priority="329">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="246" priority="330">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="expression" dxfId="244" priority="327">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="243" priority="328">
+    <cfRule type="expression" dxfId="245" priority="327">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="244" priority="328">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="242" priority="321">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="241" priority="322">
+    <cfRule type="expression" dxfId="243" priority="321">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="242" priority="322">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42">
-    <cfRule type="expression" dxfId="240" priority="319">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="239" priority="320">
+    <cfRule type="expression" dxfId="241" priority="319">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="240" priority="320">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40">
-    <cfRule type="expression" dxfId="238" priority="317">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="237" priority="318">
+    <cfRule type="expression" dxfId="239" priority="317">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="238" priority="318">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="expression" dxfId="236" priority="315">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="235" priority="316">
+    <cfRule type="expression" dxfId="237" priority="315">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="236" priority="316">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="234" priority="313">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="233" priority="314">
+    <cfRule type="expression" dxfId="235" priority="313">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="234" priority="314">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="expression" dxfId="232" priority="311">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="231" priority="312">
+    <cfRule type="expression" dxfId="233" priority="311">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="232" priority="312">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="230" priority="309">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="229" priority="310">
+    <cfRule type="expression" dxfId="231" priority="309">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="230" priority="310">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="228" priority="307">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="227" priority="308">
+    <cfRule type="expression" dxfId="229" priority="307">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="228" priority="308">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
-    <cfRule type="expression" dxfId="226" priority="305">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="225" priority="306">
+    <cfRule type="expression" dxfId="227" priority="305">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="226" priority="306">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
-    <cfRule type="expression" dxfId="224" priority="303">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="223" priority="304">
+    <cfRule type="expression" dxfId="225" priority="303">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="304">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="expression" dxfId="222" priority="301">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="221" priority="302">
+    <cfRule type="expression" dxfId="223" priority="301">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="222" priority="302">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="expression" dxfId="220" priority="299">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="219" priority="300">
+    <cfRule type="expression" dxfId="221" priority="299">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="220" priority="300">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="expression" dxfId="218" priority="287">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="217" priority="288">
+    <cfRule type="expression" dxfId="219" priority="287">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="218" priority="288">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:F44 H44:L44 N44">
-    <cfRule type="expression" dxfId="216" priority="295">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="215" priority="296">
+    <cfRule type="expression" dxfId="217" priority="295">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="216" priority="296">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="214" priority="293">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="213" priority="294">
+    <cfRule type="expression" dxfId="215" priority="293">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="214" priority="294">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="212" priority="291">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="211" priority="292">
+    <cfRule type="expression" dxfId="213" priority="291">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="212" priority="292">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="expression" dxfId="210" priority="289">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="209" priority="290">
+    <cfRule type="expression" dxfId="211" priority="289">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="210" priority="290">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45">
-    <cfRule type="expression" dxfId="208" priority="285">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="207" priority="286">
+    <cfRule type="expression" dxfId="209" priority="285">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="208" priority="286">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="206" priority="283">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="205" priority="284">
+    <cfRule type="expression" dxfId="207" priority="283">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="206" priority="284">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="204" priority="281">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="203" priority="282">
+    <cfRule type="expression" dxfId="205" priority="281">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="204" priority="282">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="202" priority="277">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="201" priority="278">
+    <cfRule type="expression" dxfId="203" priority="277">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="202" priority="278">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="200" priority="279">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="199" priority="280">
+    <cfRule type="expression" dxfId="201" priority="279">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="200" priority="280">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:N46">
-    <cfRule type="expression" dxfId="198" priority="275">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="197" priority="276">
+    <cfRule type="expression" dxfId="199" priority="275">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="198" priority="276">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q28:XFD28">
-    <cfRule type="expression" dxfId="196" priority="273">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="274">
+    <cfRule type="expression" dxfId="197" priority="273">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="196" priority="274">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="expression" dxfId="194" priority="271">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="193" priority="272">
+    <cfRule type="expression" dxfId="195" priority="271">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="194" priority="272">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="192" priority="263">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="191" priority="264">
+    <cfRule type="expression" dxfId="193" priority="263">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="192" priority="264">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N49">
-    <cfRule type="expression" dxfId="190" priority="261">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="262">
+    <cfRule type="expression" dxfId="191" priority="261">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="190" priority="262">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49">
-    <cfRule type="expression" dxfId="188" priority="259">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="187" priority="260">
+    <cfRule type="expression" dxfId="189" priority="259">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="188" priority="260">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:E49">
-    <cfRule type="expression" dxfId="186" priority="257">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="185" priority="258">
+    <cfRule type="expression" dxfId="187" priority="257">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="186" priority="258">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:B50">
-    <cfRule type="expression" dxfId="184" priority="255">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="256">
+    <cfRule type="expression" dxfId="185" priority="255">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="184" priority="256">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50">
-    <cfRule type="expression" dxfId="182" priority="247">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="181" priority="248">
+    <cfRule type="expression" dxfId="183" priority="247">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="182" priority="248">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:L50">
-    <cfRule type="expression" dxfId="180" priority="251">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="179" priority="252">
+    <cfRule type="expression" dxfId="181" priority="251">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="180" priority="252">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50">
-    <cfRule type="expression" dxfId="178" priority="249">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="250">
+    <cfRule type="expression" dxfId="179" priority="249">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="178" priority="250">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M37">
-    <cfRule type="expression" dxfId="176" priority="245">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="246">
+    <cfRule type="expression" dxfId="177" priority="245">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="176" priority="246">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51">
-    <cfRule type="expression" dxfId="174" priority="243">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="244">
+    <cfRule type="expression" dxfId="175" priority="243">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="174" priority="244">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="expression" dxfId="172" priority="241">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="171" priority="242">
+    <cfRule type="expression" dxfId="173" priority="241">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="242">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="170" priority="239">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="169" priority="240">
+    <cfRule type="expression" dxfId="171" priority="239">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="240">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51">
-    <cfRule type="expression" dxfId="168" priority="237">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="167" priority="238">
+    <cfRule type="expression" dxfId="169" priority="237">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="238">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:B52">
-    <cfRule type="expression" dxfId="166" priority="235">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="165" priority="236">
+    <cfRule type="expression" dxfId="167" priority="235">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="236">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="expression" dxfId="164" priority="233">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="163" priority="234">
+    <cfRule type="expression" dxfId="165" priority="233">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="234">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="expression" dxfId="162" priority="231">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="232">
+    <cfRule type="expression" dxfId="163" priority="231">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="232">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="160" priority="229">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="159" priority="230">
+    <cfRule type="expression" dxfId="161" priority="229">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="230">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="expression" dxfId="158" priority="223">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="224">
+    <cfRule type="expression" dxfId="159" priority="223">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="224">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52">
-    <cfRule type="expression" dxfId="156" priority="225">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="226">
+    <cfRule type="expression" dxfId="157" priority="225">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="226">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="154" priority="221">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="153" priority="222">
+    <cfRule type="expression" dxfId="155" priority="221">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="222">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="152" priority="219">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="151" priority="220">
+    <cfRule type="expression" dxfId="153" priority="219">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="220">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="expression" dxfId="150" priority="217">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="149" priority="218">
+    <cfRule type="expression" dxfId="151" priority="217">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="218">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="expression" dxfId="148" priority="215">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="147" priority="216">
+    <cfRule type="expression" dxfId="149" priority="215">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="148" priority="216">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:N53">
-    <cfRule type="expression" dxfId="146" priority="213">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="214">
+    <cfRule type="expression" dxfId="147" priority="213">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="214">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:F27 H27:K27 M27">
-    <cfRule type="expression" dxfId="144" priority="211">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="212">
+    <cfRule type="expression" dxfId="145" priority="211">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="212">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 E3:L3 N3">
-    <cfRule type="expression" dxfId="142" priority="209">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="210">
+    <cfRule type="expression" dxfId="143" priority="209">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="210">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="expression" dxfId="140" priority="207">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="208">
+    <cfRule type="expression" dxfId="141" priority="207">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="208">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="expression" dxfId="138" priority="205">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="206">
+    <cfRule type="expression" dxfId="139" priority="205">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="206">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="expression" dxfId="136" priority="203">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="204">
+    <cfRule type="expression" dxfId="137" priority="203">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="204">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="expression" dxfId="134" priority="201">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="202">
+    <cfRule type="expression" dxfId="135" priority="201">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="202">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="132" priority="199">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="200">
+    <cfRule type="expression" dxfId="133" priority="199">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="200">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:N6 D6:F6 H6:J6 M5 B5:B6">
-    <cfRule type="expression" dxfId="130" priority="197">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="198">
+    <cfRule type="expression" dxfId="131" priority="197">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="198">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="128" priority="187">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="188">
+    <cfRule type="expression" dxfId="129" priority="187">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="188">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:F5 H5:L5 N5">
-    <cfRule type="expression" dxfId="126" priority="195">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="196">
+    <cfRule type="expression" dxfId="127" priority="195">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="196">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="124" priority="193">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="123" priority="194">
+    <cfRule type="expression" dxfId="125" priority="193">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="194">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="122" priority="191">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="192">
+    <cfRule type="expression" dxfId="123" priority="191">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="192">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="expression" dxfId="120" priority="189">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="190">
+    <cfRule type="expression" dxfId="121" priority="189">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="190">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="118" priority="185">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="186">
+    <cfRule type="expression" dxfId="119" priority="185">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="186">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="116" priority="183">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="184">
+    <cfRule type="expression" dxfId="117" priority="183">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="184">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="114" priority="181">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="182">
+    <cfRule type="expression" dxfId="115" priority="181">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="182">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="112" priority="177">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="178">
+    <cfRule type="expression" dxfId="113" priority="177">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="178">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="110" priority="179">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="180">
+    <cfRule type="expression" dxfId="111" priority="179">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="180">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:N8">
-    <cfRule type="expression" dxfId="108" priority="175">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="176">
+    <cfRule type="expression" dxfId="109" priority="175">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="176">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="106" priority="161">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="162">
+    <cfRule type="expression" dxfId="107" priority="161">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="162">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="104" priority="159">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="160">
+    <cfRule type="expression" dxfId="105" priority="159">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="160">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25 M25 F25:J25">
-    <cfRule type="expression" dxfId="102" priority="158">
+    <cfRule type="expression" dxfId="103" priority="158">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25">
-    <cfRule type="expression" dxfId="101" priority="156">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="157">
+    <cfRule type="expression" dxfId="102" priority="156">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="157">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="expression" dxfId="99" priority="154">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="155">
+    <cfRule type="expression" dxfId="100" priority="154">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="155">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E25">
-    <cfRule type="expression" dxfId="97" priority="152">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="153">
+    <cfRule type="expression" dxfId="98" priority="152">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="153">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="95" priority="150">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="151">
+    <cfRule type="expression" dxfId="96" priority="150">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="151">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:F26 H26:K26 B26 M26">
-    <cfRule type="expression" dxfId="93" priority="149">
+    <cfRule type="expression" dxfId="94" priority="149">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="expression" dxfId="92" priority="147">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="148">
+    <cfRule type="expression" dxfId="93" priority="147">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="148">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="90" priority="145">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="146">
+    <cfRule type="expression" dxfId="91" priority="145">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="146">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="88" priority="143">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="144">
+    <cfRule type="expression" dxfId="89" priority="143">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="144">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="expression" dxfId="86" priority="141">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="142">
+    <cfRule type="expression" dxfId="87" priority="141">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="86" priority="142">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="expression" dxfId="84" priority="139">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="140">
+    <cfRule type="expression" dxfId="85" priority="139">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="140">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:K4 M4">
-    <cfRule type="expression" dxfId="82" priority="138">
+    <cfRule type="expression" dxfId="83" priority="138">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="expression" dxfId="81" priority="136">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="137">
+    <cfRule type="expression" dxfId="82" priority="136">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="137">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="79" priority="134">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="135">
+    <cfRule type="expression" dxfId="80" priority="134">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="135">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="77" priority="132">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="133">
+    <cfRule type="expression" dxfId="78" priority="132">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="133">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="expression" dxfId="75" priority="130">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="131">
+    <cfRule type="expression" dxfId="76" priority="130">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="131">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="expression" dxfId="73" priority="128">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="129">
+    <cfRule type="expression" dxfId="74" priority="128">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="129">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="expression" dxfId="71" priority="126">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="127">
+    <cfRule type="expression" dxfId="72" priority="126">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="127">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="expression" dxfId="69" priority="124">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="125">
+    <cfRule type="expression" dxfId="70" priority="124">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="125">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="expression" dxfId="67" priority="122">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="123">
+    <cfRule type="expression" dxfId="68" priority="122">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="123">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:J2">
-    <cfRule type="expression" dxfId="65" priority="118">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="119">
+    <cfRule type="expression" dxfId="66" priority="118">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="119">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="63" priority="107">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="108">
+    <cfRule type="expression" dxfId="64" priority="107">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="108">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="expression" dxfId="61" priority="105">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="106">
+    <cfRule type="expression" dxfId="62" priority="105">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="106">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="59" priority="97">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="98">
+    <cfRule type="expression" dxfId="60" priority="97">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="98">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="57" priority="103">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="104">
+    <cfRule type="expression" dxfId="58" priority="103">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="104">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="55" priority="101">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="102">
+    <cfRule type="expression" dxfId="56" priority="101">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="102">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="expression" dxfId="53" priority="99">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="100">
+    <cfRule type="expression" dxfId="54" priority="99">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="100">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="51" priority="95">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="96">
+    <cfRule type="expression" dxfId="52" priority="95">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="96">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="expression" dxfId="49" priority="93">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="94">
+    <cfRule type="expression" dxfId="50" priority="93">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="94">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="expression" dxfId="47" priority="85">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="86">
+    <cfRule type="expression" dxfId="48" priority="85">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="86">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="45" priority="83">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="84">
+    <cfRule type="expression" dxfId="46" priority="83">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="84">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="43" priority="81">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="82">
+    <cfRule type="expression" dxfId="44" priority="81">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="82">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="41" priority="79">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="80">
+    <cfRule type="expression" dxfId="42" priority="79">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="80">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="39" priority="77">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="78">
+    <cfRule type="expression" dxfId="40" priority="77">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="78">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="37" priority="75">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="76">
+    <cfRule type="expression" dxfId="38" priority="75">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="76">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="35" priority="73">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="74">
+    <cfRule type="expression" dxfId="36" priority="73">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="74">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:N12">
-    <cfRule type="expression" dxfId="33" priority="51">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="34" priority="51">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="52">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="expression" dxfId="31" priority="49">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="50">
+    <cfRule type="expression" dxfId="32" priority="49">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="50">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="29" priority="47">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="48">
+    <cfRule type="expression" dxfId="30" priority="47">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="48">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="expression" dxfId="27" priority="45">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="46">
+    <cfRule type="expression" dxfId="28" priority="45">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="46">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="expression" dxfId="25" priority="43">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="44">
+    <cfRule type="expression" dxfId="26" priority="43">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="44">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:E20">
-    <cfRule type="expression" dxfId="23" priority="41">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="42">
+    <cfRule type="expression" dxfId="24" priority="41">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="42">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="expression" dxfId="21" priority="33">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="34">
+    <cfRule type="expression" dxfId="22" priority="33">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:L13">
-    <cfRule type="expression" dxfId="19" priority="37">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38">
+    <cfRule type="expression" dxfId="20" priority="37">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="38">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="expression" dxfId="17" priority="35">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36">
+    <cfRule type="expression" dxfId="18" priority="35">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="36">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="expression" dxfId="15" priority="29">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="30">
+    <cfRule type="expression" dxfId="16" priority="29">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="30">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="expression" dxfId="13" priority="27">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="28">
+    <cfRule type="expression" dxfId="14" priority="27">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="28">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="11" priority="25">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="26">
+    <cfRule type="expression" dxfId="12" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="26">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="expression" dxfId="9" priority="23">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="24">
+    <cfRule type="expression" dxfId="10" priority="23">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="24">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B15">
-    <cfRule type="expression" dxfId="7" priority="21">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="22">
+    <cfRule type="expression" dxfId="8" priority="21">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="22">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="expression" dxfId="5" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="6" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="expression" dxfId="3" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="14">
+    <cfRule type="expression" dxfId="4" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:N16">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>